<commit_message>
Haldir BotF elven cloak fix
</commit_message>
<xml_diff>
--- a/data/mesbg_data.xlsx
+++ b/data/mesbg_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alex_\Downloads\mesbg-list-builder-v2024\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E157B41-F58B-4F20-B059-DABABE4B10CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2160875-BEFF-41B3-8E1E-9343A24C1D5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="models" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">hero_constraints!$A$1:$C$548</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">keywords!$A$1:$D$149</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">models!$A$1:$O$686</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">options!$A$1:$I$851</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">options!$A$1:$I$852</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">warning_rules!$A$1:$D$66</definedName>
   </definedNames>
   <calcPr calcId="191029" iterateDelta="1E-4"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10144" uniqueCount="2816">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10146" uniqueCount="2816">
   <si>
     <t>model_id</t>
   </si>
@@ -10329,7 +10329,7 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:O739"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="E1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="M111" sqref="M111"/>
@@ -43767,9 +43767,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMJ1581"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A845" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B848" sqref="B848"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A75" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C551" sqref="C551"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -58180,10 +58180,19 @@
     </row>
     <row r="852" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A852" s="23"/>
-      <c r="B852" s="23"/>
-      <c r="C852" s="20"/>
-      <c r="D852" s="20"/>
+      <c r="B852" s="13" t="s">
+        <v>207</v>
+      </c>
+      <c r="C852" s="20" t="s">
+        <v>1321</v>
+      </c>
+      <c r="D852" s="20">
+        <v>5</v>
+      </c>
       <c r="E852" s="20"/>
+      <c r="F852" s="13" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="853" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A853" s="23"/>
@@ -62729,7 +62738,7 @@
       <c r="E1581" s="20"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I851" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
+  <autoFilter ref="A1:I852" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <phoneticPr fontId="7" type="noConversion"/>
   <conditionalFormatting sqref="A1:A1048576">
     <cfRule type="duplicateValues" dxfId="3" priority="2"/>

</xml_diff>

<commit_message>
Haldir BotF cloak - free cost
</commit_message>
<xml_diff>
--- a/data/mesbg_data.xlsx
+++ b/data/mesbg_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alex_\Downloads\mesbg-list-builder-v2024\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2160875-BEFF-41B3-8E1E-9343A24C1D5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E42E0ED-D7BF-4ABD-B16E-DC104F140A21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43768,8 +43768,8 @@
   <dimension ref="A1:AMJ1581"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A75" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C551" sqref="C551"/>
+      <pane ySplit="1" topLeftCell="A845" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D853" sqref="D853"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -58187,7 +58187,7 @@
         <v>1321</v>
       </c>
       <c r="D852" s="20">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E852" s="20"/>
       <c r="F852" s="13" t="b">

</xml_diff>

<commit_message>
BotF free cloaks for all heroes
</commit_message>
<xml_diff>
--- a/data/mesbg_data.xlsx
+++ b/data/mesbg_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alex_\Downloads\mesbg-list-builder-v2024\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E42E0ED-D7BF-4ABD-B16E-DC104F140A21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03267D3C-776A-4E07-8EDA-103001809A2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10146" uniqueCount="2816">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10171" uniqueCount="2825">
   <si>
     <t>model_id</t>
   </si>
@@ -9519,6 +9519,33 @@
   </si>
   <si>
     <t>[['Arwen', '2:4:2:2'], ['Asfaloth', '0:1:1:1']]</t>
+  </si>
+  <si>
+    <t>OPT0880</t>
+  </si>
+  <si>
+    <t>OPT0881</t>
+  </si>
+  <si>
+    <t>OPT0882</t>
+  </si>
+  <si>
+    <t>OPT0883</t>
+  </si>
+  <si>
+    <t>OPT0884</t>
+  </si>
+  <si>
+    <t>OPT0885</t>
+  </si>
+  <si>
+    <t>OPT0886</t>
+  </si>
+  <si>
+    <t>OPT0887</t>
+  </si>
+  <si>
+    <t>OPT0888</t>
   </si>
 </sst>
 </file>
@@ -10329,10 +10356,10 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:O739"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="G1" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="M111" sqref="M111"/>
+      <selection pane="bottomLeft" activeCell="A68" sqref="A68:A76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -12652,7 +12679,7 @@
       </c>
       <c r="O48" s="9"/>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A49" s="9" t="s">
         <v>142</v>
       </c>
@@ -12699,7 +12726,7 @@
       </c>
       <c r="O49" s="9"/>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A50" s="9" t="s">
         <v>144</v>
       </c>
@@ -13560,7 +13587,7 @@
       </c>
       <c r="O67" s="9"/>
     </row>
-    <row r="68" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A68" s="9" t="s">
         <v>190</v>
       </c>
@@ -13607,7 +13634,7 @@
       </c>
       <c r="O68" s="9"/>
     </row>
-    <row r="69" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A69" s="9" t="s">
         <v>192</v>
       </c>
@@ -13654,7 +13681,7 @@
       </c>
       <c r="O69" s="9"/>
     </row>
-    <row r="70" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A70" s="9" t="s">
         <v>193</v>
       </c>
@@ -13701,7 +13728,7 @@
       </c>
       <c r="O70" s="9"/>
     </row>
-    <row r="71" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A71" s="9" t="s">
         <v>194</v>
       </c>
@@ -13748,7 +13775,7 @@
       </c>
       <c r="O71" s="9"/>
     </row>
-    <row r="72" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A72" s="9" t="s">
         <v>197</v>
       </c>
@@ -13795,7 +13822,7 @@
       </c>
       <c r="O72" s="9"/>
     </row>
-    <row r="73" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A73" s="9" t="s">
         <v>200</v>
       </c>
@@ -13842,7 +13869,7 @@
       </c>
       <c r="O73" s="9"/>
     </row>
-    <row r="74" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A74" s="9" t="s">
         <v>202</v>
       </c>
@@ -13889,7 +13916,7 @@
       </c>
       <c r="O74" s="9"/>
     </row>
-    <row r="75" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A75" s="9" t="s">
         <v>205</v>
       </c>
@@ -13936,7 +13963,7 @@
       </c>
       <c r="O75" s="9"/>
     </row>
-    <row r="76" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A76" s="9" t="s">
         <v>207</v>
       </c>
@@ -13983,7 +14010,7 @@
       </c>
       <c r="O76" s="9"/>
     </row>
-    <row r="77" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A77" s="9" t="s">
         <v>208</v>
       </c>
@@ -15611,7 +15638,7 @@
       </c>
       <c r="O110" s="9"/>
     </row>
-    <row r="111" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A111" s="9" t="s">
         <v>269</v>
       </c>
@@ -15802,7 +15829,7 @@
       </c>
       <c r="O114" s="9"/>
     </row>
-    <row r="115" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A115" s="9" t="s">
         <v>277</v>
       </c>
@@ -17474,7 +17501,7 @@
       </c>
       <c r="O149" s="9"/>
     </row>
-    <row r="150" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A150" s="9" t="s">
         <v>346</v>
       </c>
@@ -17568,7 +17595,7 @@
       </c>
       <c r="O151" s="9"/>
     </row>
-    <row r="152" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A152" s="9" t="s">
         <v>348</v>
       </c>
@@ -17900,7 +17927,7 @@
       </c>
       <c r="O158" s="9"/>
     </row>
-    <row r="159" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A159" s="9" t="s">
         <v>356</v>
       </c>
@@ -17994,7 +18021,7 @@
       </c>
       <c r="O160" s="9"/>
     </row>
-    <row r="161" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A161" s="9" t="s">
         <v>359</v>
       </c>
@@ -43751,10 +43778,9 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:O686" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <filterColumn colId="4">
+    <filterColumn colId="2">
       <filters>
-        <filter val="Morannon Orc Captain"/>
-        <filter val="Morannon Orc Warrior"/>
+        <filter val="Breaking of the Fellowship"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -43767,9 +43793,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMJ1581"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A845" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D853" sqref="D853"/>
+      <selection pane="bottomLeft" activeCell="B851" sqref="B851"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -58179,9 +58205,11 @@
       </c>
     </row>
     <row r="852" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A852" s="23"/>
-      <c r="B852" s="13" t="s">
-        <v>207</v>
+      <c r="A852" s="13" t="s">
+        <v>2816</v>
+      </c>
+      <c r="B852" s="9" t="s">
+        <v>190</v>
       </c>
       <c r="C852" s="20" t="s">
         <v>1321</v>
@@ -58195,60 +58223,148 @@
       </c>
     </row>
     <row r="853" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A853" s="23"/>
-      <c r="B853" s="23"/>
-      <c r="C853" s="20"/>
-      <c r="D853" s="20"/>
+      <c r="A853" s="13" t="s">
+        <v>2817</v>
+      </c>
+      <c r="B853" s="9" t="s">
+        <v>192</v>
+      </c>
+      <c r="C853" s="20" t="s">
+        <v>1321</v>
+      </c>
+      <c r="D853" s="20">
+        <v>0</v>
+      </c>
       <c r="E853" s="20"/>
+      <c r="F853" s="13" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="854" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A854" s="23"/>
-      <c r="B854" s="23"/>
-      <c r="C854" s="20"/>
-      <c r="D854" s="20"/>
+      <c r="A854" s="13" t="s">
+        <v>2818</v>
+      </c>
+      <c r="B854" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="C854" s="20" t="s">
+        <v>1321</v>
+      </c>
+      <c r="D854" s="20">
+        <v>0</v>
+      </c>
       <c r="E854" s="20"/>
+      <c r="F854" s="13" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="855" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A855" s="23"/>
-      <c r="B855" s="23"/>
-      <c r="C855" s="20"/>
-      <c r="D855" s="20"/>
+      <c r="A855" s="13" t="s">
+        <v>2819</v>
+      </c>
+      <c r="B855" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="C855" s="20" t="s">
+        <v>1321</v>
+      </c>
+      <c r="D855" s="20">
+        <v>0</v>
+      </c>
       <c r="E855" s="20"/>
+      <c r="F855" s="13" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="856" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A856" s="23"/>
-      <c r="B856" s="23"/>
-      <c r="C856" s="20"/>
-      <c r="D856" s="20"/>
+      <c r="A856" s="13" t="s">
+        <v>2820</v>
+      </c>
+      <c r="B856" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="C856" s="20" t="s">
+        <v>1321</v>
+      </c>
+      <c r="D856" s="20">
+        <v>0</v>
+      </c>
       <c r="E856" s="20"/>
+      <c r="F856" s="13" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="857" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A857" s="23"/>
-      <c r="B857" s="23"/>
-      <c r="C857" s="20"/>
-      <c r="D857" s="20"/>
+      <c r="A857" s="13" t="s">
+        <v>2821</v>
+      </c>
+      <c r="B857" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="C857" s="20" t="s">
+        <v>1321</v>
+      </c>
+      <c r="D857" s="20">
+        <v>0</v>
+      </c>
       <c r="E857" s="20"/>
+      <c r="F857" s="13" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="858" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A858" s="23"/>
-      <c r="B858" s="23"/>
-      <c r="C858" s="20"/>
-      <c r="D858" s="20"/>
+      <c r="A858" s="13" t="s">
+        <v>2822</v>
+      </c>
+      <c r="B858" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="C858" s="20" t="s">
+        <v>1321</v>
+      </c>
+      <c r="D858" s="20">
+        <v>0</v>
+      </c>
       <c r="E858" s="20"/>
+      <c r="F858" s="13" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="859" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A859" s="23"/>
-      <c r="B859" s="23"/>
-      <c r="C859" s="20"/>
-      <c r="D859" s="20"/>
+      <c r="A859" s="13" t="s">
+        <v>2823</v>
+      </c>
+      <c r="B859" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="C859" s="20" t="s">
+        <v>1321</v>
+      </c>
+      <c r="D859" s="20">
+        <v>0</v>
+      </c>
       <c r="E859" s="20"/>
+      <c r="F859" s="13" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="860" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A860" s="23"/>
-      <c r="B860" s="23"/>
-      <c r="C860" s="20"/>
-      <c r="D860" s="20"/>
+      <c r="A860" s="13" t="s">
+        <v>2824</v>
+      </c>
+      <c r="B860" s="9" t="s">
+        <v>207</v>
+      </c>
+      <c r="C860" s="20" t="s">
+        <v>1321</v>
+      </c>
+      <c r="D860" s="20">
+        <v>0</v>
+      </c>
       <c r="E860" s="20"/>
+      <c r="F860" s="13" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="861" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A861" s="23"/>

</xml_diff>